<commit_message>
add: desenvolvimento avaliacao heuristicas
</commit_message>
<xml_diff>
--- a/Trabalho3/Entrega2/AvaliacaoHeuristica.xlsx
+++ b/Trabalho3/Entrega2/AvaliacaoHeuristica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus Caçabuena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus Caçabuena\Desktop\estudos\pucrs\ExperienciaDoUsuario\Trabalho3\Entrega2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2988FD0-9F5B-4414-81F3-17F7A2FCBADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D274E-E38C-4E30-8A25-E24960FC8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C5DD57C8-0B84-458E-9237-08286E66ECD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5DD57C8-0B84-458E-9237-08286E66ECD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Carolina Ferreira" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="13">
   <si>
     <t>Tela Principal</t>
   </si>
@@ -57,6 +57,27 @@
   </si>
   <si>
     <t>Heurísticas</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2 - limpar filtros</t>
+  </si>
+  <si>
+    <t>5 - confirmar filtro</t>
+  </si>
+  <si>
+    <t>9 - sem resultados</t>
+  </si>
+  <si>
+    <t>9 - erro de envio</t>
+  </si>
+  <si>
+    <t>3 - desinscrever</t>
+  </si>
+  <si>
+    <t>5 - conf. presença</t>
   </si>
 </sst>
 </file>
@@ -408,19 +429,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF73731-DE94-42F5-985A-EC0B01BCFC2C}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -450,29 +471,119 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -480,20 +591,101 @@
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF60888-4A56-4204-99B5-755D470DD8A1}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>